<commit_message>
Image path updated of alumni in sheet
</commit_message>
<xml_diff>
--- a/alumni.xlsx
+++ b/alumni.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058DC641-2E33-4D85-ADCE-B105FBE4DF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADB6991-CFFC-4C7D-B90A-B4B95F316E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,156 +45,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>https://placehold.co/600x400</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x401</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x402</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x403</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x404</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x405</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x406</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x407</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x408</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x409</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x410</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x411</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x412</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x413</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x414</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x415</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x416</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x417</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x418</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x419</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x420</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x421</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x422</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x423</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x424</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x425</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x426</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x427</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x428</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x429</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x430</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x431</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x432</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x433</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x434</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x435</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x436</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x437</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x438</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x439</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x440</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x441</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x442</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x443</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x444</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x445</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x446</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x447</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x448</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x449</t>
-  </si>
-  <si>
     <t>Mr. Divyanshu Bhatt</t>
   </si>
   <si>
@@ -670,21 +520,6 @@
     <t>Energy (Enkon Energy Advisors Llc – Houston, Texas</t>
   </si>
   <si>
-    <t>https://placehold.co/600x450</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x451</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x452</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x453</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x454</t>
-  </si>
-  <si>
     <t>Department of Defence with ACE contractors, Melbourne</t>
   </si>
   <si>
@@ -692,6 +527,171 @@
   </si>
   <si>
     <t>Ministry Of Defence, Govt. Of India.</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Divyansh_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Parth_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Zaheen_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Divya_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Upasana_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Kushal_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Chintan_Cl.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Neha_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Rushit_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Pranay_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Yash_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Dhruval_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Abhishek_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Nishil_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Chetan_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Himil_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Mohil_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Yaydeep_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Smit_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Payal_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Jignesh_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Jugal_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Hirak_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Vidhi_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Ashish_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Yash_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Malay_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Dhaivat_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\AbhishekSingh_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Riya_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\08EC089_Mayank_Patel.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\Parthav Pankaj Vyas.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\Nilesh Ranpura.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\09EC035_Harshita_Joshi.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\Kishan_Portrait_pic.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Shashin_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Vivek_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Tadarsh_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Kaushal_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Namra_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Prince_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Forum_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Utsav_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Rutu_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Mansi_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\1. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\2. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\3. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\4. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\5. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\6. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\7. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\8. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\9. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\10. ALUMNI IMAGE.webp</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,774 +1082,774 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>218</v>
+        <v>163</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>217</v>
+        <v>162</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>27</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>35</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>37</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>40</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>42</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>44</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>46</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>48</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>49</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>50</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>51</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>52</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>219</v>
+        <v>164</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>53</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>54</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1857,12 +1857,60 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{549F0858-9767-470C-A713-55C60B01FFD3}"/>
     <hyperlink ref="D3:D51" r:id="rId2" display="https://placehold.co/600x400" xr:uid="{8B094356-DB52-4055-8E33-7DD1BE21E804}"/>
-    <hyperlink ref="D51" r:id="rId3" display="https://placehold.co/600x400" xr:uid="{0FB08AC4-1313-4706-861B-0CD1D7C4BB5B}"/>
-    <hyperlink ref="D52" r:id="rId4" display="https://placehold.co/600x400" xr:uid="{27FD5750-98B7-4EA2-A474-7A20D523393A}"/>
-    <hyperlink ref="D53" r:id="rId5" display="https://placehold.co/600x400" xr:uid="{559F47A5-6987-4A22-93CF-F26BDEC14FA5}"/>
-    <hyperlink ref="D54" r:id="rId6" display="https://placehold.co/600x400" xr:uid="{77071A68-BC43-411A-ABA4-82FC7E10D817}"/>
-    <hyperlink ref="D55" r:id="rId7" display="https://placehold.co/600x400" xr:uid="{D46F0146-6788-4018-B41E-84D46D7B883D}"/>
-    <hyperlink ref="D56" r:id="rId8" display="https://placehold.co/600x400" xr:uid="{FD2283D0-E7A2-4B1A-82F8-2475DEFCAC7B}"/>
+    <hyperlink ref="D51" r:id="rId3" xr:uid="{0FB08AC4-1313-4706-861B-0CD1D7C4BB5B}"/>
+    <hyperlink ref="D52" r:id="rId4" xr:uid="{27FD5750-98B7-4EA2-A474-7A20D523393A}"/>
+    <hyperlink ref="D53" r:id="rId5" xr:uid="{559F47A5-6987-4A22-93CF-F26BDEC14FA5}"/>
+    <hyperlink ref="D54" r:id="rId6" xr:uid="{77071A68-BC43-411A-ABA4-82FC7E10D817}"/>
+    <hyperlink ref="D55" r:id="rId7" xr:uid="{D46F0146-6788-4018-B41E-84D46D7B883D}"/>
+    <hyperlink ref="D56" r:id="rId8" xr:uid="{FD2283D0-E7A2-4B1A-82F8-2475DEFCAC7B}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{AEAB1B0C-3985-4180-83EA-4C5515B48A64}"/>
+    <hyperlink ref="D4" r:id="rId10" xr:uid="{5EF259C6-2B01-4C16-8D2B-AAF4398D111B}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{693F7013-3DFB-47EE-9015-7880DE23E944}"/>
+    <hyperlink ref="D6" r:id="rId12" xr:uid="{BA48C03E-FD9C-4E7F-9CB2-A2B9B28C5033}"/>
+    <hyperlink ref="D7" r:id="rId13" xr:uid="{7EDB5851-CC53-431C-B1B7-05C542E6BD5E}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{204A4B62-E6CB-49BC-8053-59946CFE8BCA}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{ACD4AD6C-BCEA-4B8A-8B99-0C0D37CB831A}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{081CFFD6-A64A-4BE0-8674-70615741BD75}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{A1DBA03A-17C8-4CF3-85C4-5EDD26E18F6F}"/>
+    <hyperlink ref="D12" r:id="rId18" xr:uid="{ECAC2F85-1FCB-4746-A24B-09DBD5C7EB87}"/>
+    <hyperlink ref="D13" r:id="rId19" xr:uid="{5C59E1A9-B129-4DE7-A1D4-68B9FB3AF77A}"/>
+    <hyperlink ref="D14" r:id="rId20" xr:uid="{F16F7D62-5000-4D8E-BF20-16CE6DE00E6E}"/>
+    <hyperlink ref="D15" r:id="rId21" xr:uid="{D837CA59-74B5-4285-9D63-6F250566DB32}"/>
+    <hyperlink ref="D16" r:id="rId22" xr:uid="{781DCD30-6FF4-4CEB-9E87-D1F6F0BDDDF6}"/>
+    <hyperlink ref="D17" r:id="rId23" xr:uid="{CE923F85-412E-4662-8C2F-42141836159D}"/>
+    <hyperlink ref="D18" r:id="rId24" xr:uid="{00240428-3671-41C3-B724-CBD05AADE392}"/>
+    <hyperlink ref="D19" r:id="rId25" xr:uid="{8D374A50-1528-4392-B977-16F689F2056F}"/>
+    <hyperlink ref="D20" r:id="rId26" xr:uid="{83D994FC-391C-4C29-9CA9-AADF3CCE8752}"/>
+    <hyperlink ref="D21" r:id="rId27" xr:uid="{B711232B-BDF8-4D50-9B71-6C92AF7F231E}"/>
+    <hyperlink ref="D22" r:id="rId28" xr:uid="{6B66BCB9-0836-4BE9-BCCA-E6402D05AC2B}"/>
+    <hyperlink ref="D23" r:id="rId29" xr:uid="{ABF26ECE-DE10-43A0-B8F3-2B2FD149A53A}"/>
+    <hyperlink ref="D24" r:id="rId30" xr:uid="{034C49EE-5B30-4F34-B98C-69DDDBFD2CD5}"/>
+    <hyperlink ref="D25" r:id="rId31" xr:uid="{787E196C-2F95-49A2-8953-59C01EDDB445}"/>
+    <hyperlink ref="D26" r:id="rId32" xr:uid="{BED0377C-E198-47DA-B6B1-C92A516EF1DB}"/>
+    <hyperlink ref="D27" r:id="rId33" xr:uid="{902709C9-01BF-4FFA-88ED-2D96A7038677}"/>
+    <hyperlink ref="D28" r:id="rId34" xr:uid="{4FE78FB6-E21F-41F9-ABFC-674852164577}"/>
+    <hyperlink ref="D29" r:id="rId35" xr:uid="{DBD428FF-3186-41C9-BB22-816294880A19}"/>
+    <hyperlink ref="D30" r:id="rId36" xr:uid="{2C8EA120-8F36-4062-871C-E3ED9D125915}"/>
+    <hyperlink ref="D31" r:id="rId37" xr:uid="{4FE68482-E000-49C1-B061-8120F635D7F0}"/>
+    <hyperlink ref="D32" r:id="rId38" xr:uid="{56ADB5FE-18ED-4580-9F3F-96A97DC4429C}"/>
+    <hyperlink ref="D33" r:id="rId39" xr:uid="{EF59312B-6B71-4022-9505-F652F9872D9D}"/>
+    <hyperlink ref="D34" r:id="rId40" xr:uid="{B36791F9-8DB5-431F-9F74-FA52EEA1710C}"/>
+    <hyperlink ref="D35" r:id="rId41" xr:uid="{2BF83471-7103-4670-8686-99BD848615BE}"/>
+    <hyperlink ref="D36" r:id="rId42" xr:uid="{7D3F2B50-C3DC-4BE5-B76E-13638F116328}"/>
+    <hyperlink ref="D37" r:id="rId43" xr:uid="{73361DED-F53C-48EA-B59D-E8D07A7A2936}"/>
+    <hyperlink ref="D38" r:id="rId44" xr:uid="{1198048B-E67F-4F71-A452-9C73B6509DCF}"/>
+    <hyperlink ref="D39" r:id="rId45" xr:uid="{ED73140A-3692-40D7-B0CB-B620177F61A1}"/>
+    <hyperlink ref="D40" r:id="rId46" xr:uid="{99C888F0-7A87-43B1-8E47-12F249FFD261}"/>
+    <hyperlink ref="D41" r:id="rId47" xr:uid="{EE28E699-F761-4E1C-A1FF-93C35AB7B0B6}"/>
+    <hyperlink ref="D42" r:id="rId48" xr:uid="{E3A94729-A0CD-466B-B752-A9FDF2E61140}"/>
+    <hyperlink ref="D43" r:id="rId49" xr:uid="{643BF3B8-B431-4FFE-8D43-8B3A031142CF}"/>
+    <hyperlink ref="D44" r:id="rId50" xr:uid="{49211B47-743F-4550-BB4A-A53FF4957AF7}"/>
+    <hyperlink ref="D45" r:id="rId51" xr:uid="{F7483BC7-829E-48E7-B647-684008D2A45C}"/>
+    <hyperlink ref="D46" r:id="rId52" xr:uid="{9B115917-C040-409D-9E47-32D0B99708E2}"/>
+    <hyperlink ref="D47" r:id="rId53" xr:uid="{3788789B-15BE-4BB4-BFB6-09321E31B726}"/>
+    <hyperlink ref="D48" r:id="rId54" xr:uid="{AE84B85A-768D-4AD2-AB02-541C75E5792F}"/>
+    <hyperlink ref="D49" r:id="rId55" xr:uid="{8372F162-B276-401D-BFAF-C2FF656952D7}"/>
+    <hyperlink ref="D50" r:id="rId56" xr:uid="{323C6D1B-1DA2-48C5-8BC7-F0AFB8A985B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
alumni section added and commented
</commit_message>
<xml_diff>
--- a/alumni.xlsx
+++ b/alumni.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058DC641-2E33-4D85-ADCE-B105FBE4DF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADB6991-CFFC-4C7D-B90A-B4B95F316E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,156 +45,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>https://placehold.co/600x400</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x401</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x402</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x403</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x404</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x405</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x406</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x407</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x408</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x409</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x410</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x411</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x412</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x413</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x414</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x415</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x416</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x417</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x418</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x419</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x420</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x421</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x422</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x423</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x424</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x425</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x426</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x427</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x428</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x429</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x430</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x431</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x432</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x433</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x434</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x435</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x436</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x437</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x438</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x439</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x440</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x441</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x442</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x443</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x444</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x445</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x446</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x447</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x448</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x449</t>
-  </si>
-  <si>
     <t>Mr. Divyanshu Bhatt</t>
   </si>
   <si>
@@ -670,21 +520,6 @@
     <t>Energy (Enkon Energy Advisors Llc – Houston, Texas</t>
   </si>
   <si>
-    <t>https://placehold.co/600x450</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x451</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x452</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x453</t>
-  </si>
-  <si>
-    <t>https://placehold.co/600x454</t>
-  </si>
-  <si>
     <t>Department of Defence with ACE contractors, Melbourne</t>
   </si>
   <si>
@@ -692,6 +527,171 @@
   </si>
   <si>
     <t>Ministry Of Defence, Govt. Of India.</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Divyansh_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Parth_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Zaheen_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Divya_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Upasana_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Kushal_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Chintan_Cl.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Neha_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Rushit_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Pranay_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CL\Yash_CL.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Dhruval_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Abhishek_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Nishil_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Chetan_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Himil_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Mohil_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Yaydeep_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Smit_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Payal_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Jignesh_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Jugal_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Hirak_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Vidhi_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Ashish_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Yash_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Malay_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Dhaivat_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\AbhishekSingh_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EE\Riya_EE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\08EC089_Mayank_Patel.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\Parthav Pankaj Vyas.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\Nilesh Ranpura.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\09EC035_Harshita_Joshi.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\EC\Kishan_Portrait_pic.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Shashin_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Vivek_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Tadarsh_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Kaushal_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Namra_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Prince_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Forum_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Utsav_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Rutu_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\CE\Mansi_CE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\1. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\2. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\3. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\4. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\5. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\6. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\7. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\8. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\9. ALUMNI IMAGE.webp</t>
+  </si>
+  <si>
+    <t>images1\Alumni\ME\10. ALUMNI IMAGE.webp</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,774 +1082,774 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>218</v>
+        <v>163</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>217</v>
+        <v>162</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>27</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>35</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>37</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>40</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>42</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>44</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>46</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>48</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>49</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>50</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>51</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>52</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>219</v>
+        <v>164</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>53</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>54</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1857,12 +1857,60 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{549F0858-9767-470C-A713-55C60B01FFD3}"/>
     <hyperlink ref="D3:D51" r:id="rId2" display="https://placehold.co/600x400" xr:uid="{8B094356-DB52-4055-8E33-7DD1BE21E804}"/>
-    <hyperlink ref="D51" r:id="rId3" display="https://placehold.co/600x400" xr:uid="{0FB08AC4-1313-4706-861B-0CD1D7C4BB5B}"/>
-    <hyperlink ref="D52" r:id="rId4" display="https://placehold.co/600x400" xr:uid="{27FD5750-98B7-4EA2-A474-7A20D523393A}"/>
-    <hyperlink ref="D53" r:id="rId5" display="https://placehold.co/600x400" xr:uid="{559F47A5-6987-4A22-93CF-F26BDEC14FA5}"/>
-    <hyperlink ref="D54" r:id="rId6" display="https://placehold.co/600x400" xr:uid="{77071A68-BC43-411A-ABA4-82FC7E10D817}"/>
-    <hyperlink ref="D55" r:id="rId7" display="https://placehold.co/600x400" xr:uid="{D46F0146-6788-4018-B41E-84D46D7B883D}"/>
-    <hyperlink ref="D56" r:id="rId8" display="https://placehold.co/600x400" xr:uid="{FD2283D0-E7A2-4B1A-82F8-2475DEFCAC7B}"/>
+    <hyperlink ref="D51" r:id="rId3" xr:uid="{0FB08AC4-1313-4706-861B-0CD1D7C4BB5B}"/>
+    <hyperlink ref="D52" r:id="rId4" xr:uid="{27FD5750-98B7-4EA2-A474-7A20D523393A}"/>
+    <hyperlink ref="D53" r:id="rId5" xr:uid="{559F47A5-6987-4A22-93CF-F26BDEC14FA5}"/>
+    <hyperlink ref="D54" r:id="rId6" xr:uid="{77071A68-BC43-411A-ABA4-82FC7E10D817}"/>
+    <hyperlink ref="D55" r:id="rId7" xr:uid="{D46F0146-6788-4018-B41E-84D46D7B883D}"/>
+    <hyperlink ref="D56" r:id="rId8" xr:uid="{FD2283D0-E7A2-4B1A-82F8-2475DEFCAC7B}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{AEAB1B0C-3985-4180-83EA-4C5515B48A64}"/>
+    <hyperlink ref="D4" r:id="rId10" xr:uid="{5EF259C6-2B01-4C16-8D2B-AAF4398D111B}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{693F7013-3DFB-47EE-9015-7880DE23E944}"/>
+    <hyperlink ref="D6" r:id="rId12" xr:uid="{BA48C03E-FD9C-4E7F-9CB2-A2B9B28C5033}"/>
+    <hyperlink ref="D7" r:id="rId13" xr:uid="{7EDB5851-CC53-431C-B1B7-05C542E6BD5E}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{204A4B62-E6CB-49BC-8053-59946CFE8BCA}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{ACD4AD6C-BCEA-4B8A-8B99-0C0D37CB831A}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{081CFFD6-A64A-4BE0-8674-70615741BD75}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{A1DBA03A-17C8-4CF3-85C4-5EDD26E18F6F}"/>
+    <hyperlink ref="D12" r:id="rId18" xr:uid="{ECAC2F85-1FCB-4746-A24B-09DBD5C7EB87}"/>
+    <hyperlink ref="D13" r:id="rId19" xr:uid="{5C59E1A9-B129-4DE7-A1D4-68B9FB3AF77A}"/>
+    <hyperlink ref="D14" r:id="rId20" xr:uid="{F16F7D62-5000-4D8E-BF20-16CE6DE00E6E}"/>
+    <hyperlink ref="D15" r:id="rId21" xr:uid="{D837CA59-74B5-4285-9D63-6F250566DB32}"/>
+    <hyperlink ref="D16" r:id="rId22" xr:uid="{781DCD30-6FF4-4CEB-9E87-D1F6F0BDDDF6}"/>
+    <hyperlink ref="D17" r:id="rId23" xr:uid="{CE923F85-412E-4662-8C2F-42141836159D}"/>
+    <hyperlink ref="D18" r:id="rId24" xr:uid="{00240428-3671-41C3-B724-CBD05AADE392}"/>
+    <hyperlink ref="D19" r:id="rId25" xr:uid="{8D374A50-1528-4392-B977-16F689F2056F}"/>
+    <hyperlink ref="D20" r:id="rId26" xr:uid="{83D994FC-391C-4C29-9CA9-AADF3CCE8752}"/>
+    <hyperlink ref="D21" r:id="rId27" xr:uid="{B711232B-BDF8-4D50-9B71-6C92AF7F231E}"/>
+    <hyperlink ref="D22" r:id="rId28" xr:uid="{6B66BCB9-0836-4BE9-BCCA-E6402D05AC2B}"/>
+    <hyperlink ref="D23" r:id="rId29" xr:uid="{ABF26ECE-DE10-43A0-B8F3-2B2FD149A53A}"/>
+    <hyperlink ref="D24" r:id="rId30" xr:uid="{034C49EE-5B30-4F34-B98C-69DDDBFD2CD5}"/>
+    <hyperlink ref="D25" r:id="rId31" xr:uid="{787E196C-2F95-49A2-8953-59C01EDDB445}"/>
+    <hyperlink ref="D26" r:id="rId32" xr:uid="{BED0377C-E198-47DA-B6B1-C92A516EF1DB}"/>
+    <hyperlink ref="D27" r:id="rId33" xr:uid="{902709C9-01BF-4FFA-88ED-2D96A7038677}"/>
+    <hyperlink ref="D28" r:id="rId34" xr:uid="{4FE78FB6-E21F-41F9-ABFC-674852164577}"/>
+    <hyperlink ref="D29" r:id="rId35" xr:uid="{DBD428FF-3186-41C9-BB22-816294880A19}"/>
+    <hyperlink ref="D30" r:id="rId36" xr:uid="{2C8EA120-8F36-4062-871C-E3ED9D125915}"/>
+    <hyperlink ref="D31" r:id="rId37" xr:uid="{4FE68482-E000-49C1-B061-8120F635D7F0}"/>
+    <hyperlink ref="D32" r:id="rId38" xr:uid="{56ADB5FE-18ED-4580-9F3F-96A97DC4429C}"/>
+    <hyperlink ref="D33" r:id="rId39" xr:uid="{EF59312B-6B71-4022-9505-F652F9872D9D}"/>
+    <hyperlink ref="D34" r:id="rId40" xr:uid="{B36791F9-8DB5-431F-9F74-FA52EEA1710C}"/>
+    <hyperlink ref="D35" r:id="rId41" xr:uid="{2BF83471-7103-4670-8686-99BD848615BE}"/>
+    <hyperlink ref="D36" r:id="rId42" xr:uid="{7D3F2B50-C3DC-4BE5-B76E-13638F116328}"/>
+    <hyperlink ref="D37" r:id="rId43" xr:uid="{73361DED-F53C-48EA-B59D-E8D07A7A2936}"/>
+    <hyperlink ref="D38" r:id="rId44" xr:uid="{1198048B-E67F-4F71-A452-9C73B6509DCF}"/>
+    <hyperlink ref="D39" r:id="rId45" xr:uid="{ED73140A-3692-40D7-B0CB-B620177F61A1}"/>
+    <hyperlink ref="D40" r:id="rId46" xr:uid="{99C888F0-7A87-43B1-8E47-12F249FFD261}"/>
+    <hyperlink ref="D41" r:id="rId47" xr:uid="{EE28E699-F761-4E1C-A1FF-93C35AB7B0B6}"/>
+    <hyperlink ref="D42" r:id="rId48" xr:uid="{E3A94729-A0CD-466B-B752-A9FDF2E61140}"/>
+    <hyperlink ref="D43" r:id="rId49" xr:uid="{643BF3B8-B431-4FFE-8D43-8B3A031142CF}"/>
+    <hyperlink ref="D44" r:id="rId50" xr:uid="{49211B47-743F-4550-BB4A-A53FF4957AF7}"/>
+    <hyperlink ref="D45" r:id="rId51" xr:uid="{F7483BC7-829E-48E7-B647-684008D2A45C}"/>
+    <hyperlink ref="D46" r:id="rId52" xr:uid="{9B115917-C040-409D-9E47-32D0B99708E2}"/>
+    <hyperlink ref="D47" r:id="rId53" xr:uid="{3788789B-15BE-4BB4-BFB6-09321E31B726}"/>
+    <hyperlink ref="D48" r:id="rId54" xr:uid="{AE84B85A-768D-4AD2-AB02-541C75E5792F}"/>
+    <hyperlink ref="D49" r:id="rId55" xr:uid="{8372F162-B276-401D-BFAF-C2FF656952D7}"/>
+    <hyperlink ref="D50" r:id="rId56" xr:uid="{323C6D1B-1DA2-48C5-8BC7-F0AFB8A985B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>